<commit_message>
some user control methods
</commit_message>
<xml_diff>
--- a/wepAplication/webAplication/Files/report.xlsx
+++ b/wepAplication/webAplication/Files/report.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>Меню: Завтрак</t>
   </si>
@@ -30,6 +30,12 @@
   </si>
   <si>
     <t>Всего</t>
+  </si>
+  <si>
+    <t>Артем</t>
+  </si>
+  <si>
+    <t>чай</t>
   </si>
 </sst>
 </file>
@@ -51,7 +57,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -61,15 +67,43 @@
     </border>
     <border>
       <left/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
+      <right/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
       <bottom style="thin"/>
       <diagonal/>
     </border>
@@ -84,16 +118,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyProtection="1"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" xfId="0" applyProtection="1"/>
-    <xf numFmtId="0" fontId="0" borderId="1" applyBorder="1" applyProtection="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" borderId="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" borderId="2" applyBorder="1" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" borderId="3" applyBorder="1" applyProtection="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="3" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" borderId="4" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" borderId="5" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" borderId="6" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" borderId="7" applyBorder="1" applyProtection="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -106,7 +144,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="xr">
-  <dimension ref="B2:O3"/>
+  <dimension ref="B2:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -127,50 +165,68 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2"/>
-      <c r="G2" s="2" t="s">
+      <c r="C2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="H2" s="2"/>
-      <c r="L2" s="2" t="s">
+      <c r="H2" s="3"/>
+      <c r="L2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="2"/>
+      <c r="M2" s="3"/>
     </row>
     <row r="3">
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="G3" s="3" t="s">
+      <c r="E3" s="2"/>
+      <c r="G3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="I3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="J3" s="1"/>
-      <c r="L3" s="3" t="s">
+      <c r="J3" s="2"/>
+      <c r="L3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="M3" s="3" t="s">
+      <c r="M3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="N3" s="4" t="s">
+      <c r="N3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="O3" s="1"/>
+      <c r="O3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="B4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
     </row>
   </sheetData>
   <mergeCells>

</xml_diff>